<commit_message>
Deploying to gh-pages from @ TopologyHealth/IG-Authoring-Prompts@5938a207b35c2d5553bb5b7724fe9b9a368bf30f 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-MyPatient.xlsx
+++ b/StructureDefinition-MyPatient.xlsx
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-08-26T20:22:10+00:00</t>
+    <t>2025-09-18T12:32:11+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -365,7 +365,7 @@
     <t>A human language.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/languages</t>
+    <t>http://hl7.org/fhir/ValueSet/languages|4.0.1</t>
   </si>
   <si>
     <t>Resource.language</t>
@@ -750,7 +750,7 @@
     <t>The domestic partnership status of a person.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/marital-status</t>
+    <t>http://hl7.org/fhir/ValueSet/marital-status|4.0.1</t>
   </si>
   <si>
     <t>player[classCode=PSN]/maritalStatusCode</t>
@@ -901,7 +901,7 @@
     <t>The nature of the relationship between a patient and a contact person for that patient.</t>
   </si>
   <si>
-    <t>http://hl7.org/fhir/ValueSet/patient-contactrelationship</t>
+    <t>http://hl7.org/fhir/ValueSet/patient-contactrelationship|4.0.1</t>
   </si>
   <si>
     <t>code</t>
@@ -970,7 +970,7 @@
     <t>Patient.contact.organization</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Organization)
+    <t xml:space="preserve">Reference(Organization|4.0.1)
 </t>
   </si>
   <si>
@@ -1094,7 +1094,7 @@
 </t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Organization|Practitioner|PractitionerRole)
+    <t xml:space="preserve">Reference(Organization|4.0.1|Practitioner|4.0.1|PractitionerRole|4.0.1)
 </t>
   </si>
   <si>
@@ -1165,7 +1165,7 @@
     <t>Patient.link.other</t>
   </si>
   <si>
-    <t xml:space="preserve">Reference(Patient|RelatedPerson)
+    <t xml:space="preserve">Reference(Patient|4.0.1|RelatedPerson|4.0.1)
 </t>
   </si>
   <si>
@@ -1545,7 +1545,7 @@
     <col min="23" max="23" width="16.3203125" customWidth="true" bestFit="true"/>
     <col min="24" max="24" width="16.16796875" customWidth="true" bestFit="true"/>
     <col min="25" max="25" width="69.35546875" customWidth="true" bestFit="true"/>
-    <col min="26" max="26" width="44.51171875" customWidth="true" bestFit="true"/>
+    <col min="26" max="26" width="48.33203125" customWidth="true" bestFit="true"/>
     <col min="27" max="27" width="5.44140625" customWidth="true" bestFit="true"/>
     <col min="28" max="28" width="19.4765625" customWidth="true" bestFit="true"/>
     <col min="29" max="29" width="17.65625" customWidth="true" bestFit="true"/>

</xml_diff>